<commit_message>
toevoegen van dfKalender en functie OpdachtUitvoeren
</commit_message>
<xml_diff>
--- a/MODPRdataset.xlsx
+++ b/MODPRdataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robbert\Github\Modelleren\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{316D6261-6E41-4DB7-84A1-353303E22C8A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D1D9AC-3A75-4900-91F9-8EF943C1283B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{24CE0B4A-80F4-8A44-8D6D-9FAD261C3CF8}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1766" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1750" uniqueCount="428">
   <si>
     <t>Task</t>
   </si>
@@ -1044,12 +1044,6 @@
     <t>must have acquired skill 8 by the end of sprint 4</t>
   </si>
   <si>
-    <t>hiring should be kept to a minimum; hired workers can only be assigned to project tasks</t>
-  </si>
-  <si>
-    <t>costs depend on duration of assigned tasks and skills of hired worker</t>
-  </si>
-  <si>
     <t>base cost</t>
   </si>
   <si>
@@ -1089,19 +1083,10 @@
     <t>skill 13</t>
   </si>
   <si>
-    <t>hired workers have skills 1 and 8</t>
-  </si>
-  <si>
-    <t>'short' means duration of assigned tasks is at most 60 hours in total</t>
-  </si>
-  <si>
     <t>short</t>
   </si>
   <si>
     <t>other</t>
-  </si>
-  <si>
-    <t>hourly costs</t>
   </si>
   <si>
     <t>+5</t>
@@ -1750,61 +1735,61 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>427</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>432</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>92</v>
@@ -3588,13 +3573,13 @@
         <v>6</v>
       </c>
       <c r="X1" s="4" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="Y1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="Z1" s="4" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
@@ -3617,7 +3602,7 @@
         <v>96</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="I2">
         <v>8</v>
@@ -7455,7 +7440,7 @@
     </row>
     <row r="229" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A229" s="4" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="K229" t="s">
         <v>22</v>
@@ -7485,7 +7470,7 @@
     </row>
     <row r="230" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A230" s="4" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="K230" t="s">
         <v>22</v>
@@ -7513,7 +7498,7 @@
     </row>
     <row r="231" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A231" s="4" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="K231" t="s">
         <v>22</v>
@@ -7541,7 +7526,7 @@
     </row>
     <row r="232" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A232" s="4" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="K232" t="s">
         <v>22</v>
@@ -7619,7 +7604,7 @@
     </row>
     <row r="236" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A236" s="4" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="K236" t="s">
         <v>22</v>
@@ -7649,7 +7634,7 @@
     </row>
     <row r="237" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A237" s="4" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="K237" t="s">
         <v>22</v>
@@ -7677,7 +7662,7 @@
     </row>
     <row r="238" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A238" s="4" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="K238" t="s">
         <v>22</v>
@@ -7705,7 +7690,7 @@
     </row>
     <row r="239" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A239" s="4" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="K239" t="s">
         <v>22</v>
@@ -7733,7 +7718,7 @@
     </row>
     <row r="240" spans="1:26" ht="112.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" s="4" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="K240" t="s">
         <v>22</v>
@@ -7741,7 +7726,7 @@
       <c r="O240" s="4"/>
       <c r="T240" s="1"/>
       <c r="U240" s="5" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="V240" s="4" t="s">
         <v>30</v>
@@ -7759,7 +7744,7 @@
     </row>
     <row r="241" spans="1:26" ht="112.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="4" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="K241" t="s">
         <v>22</v>
@@ -7767,7 +7752,7 @@
       <c r="O241" s="4"/>
       <c r="T241" s="1"/>
       <c r="U241" s="5" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="V241" s="4" t="s">
         <v>30</v>
@@ -7785,7 +7770,7 @@
     </row>
     <row r="242" spans="1:26" ht="112.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="4" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="K242" t="s">
         <v>22</v>
@@ -7793,7 +7778,7 @@
       <c r="O242" s="4"/>
       <c r="T242" s="1"/>
       <c r="U242" s="5" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="V242" s="4" t="s">
         <v>30</v>
@@ -7811,7 +7796,7 @@
     </row>
     <row r="243" spans="1:26" ht="112.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="4" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="K243" t="s">
         <v>22</v>
@@ -7819,7 +7804,7 @@
       <c r="O243" s="4"/>
       <c r="T243" s="1"/>
       <c r="U243" s="5" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="V243" s="4" t="s">
         <v>30</v>
@@ -7837,7 +7822,7 @@
     </row>
     <row r="244" spans="1:26" ht="112.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A244" s="4" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="L244" t="s">
         <v>22</v>
@@ -7845,7 +7830,7 @@
       <c r="O244" s="4"/>
       <c r="T244" s="1"/>
       <c r="U244" s="5" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="V244" s="4" t="s">
         <v>276</v>
@@ -7860,7 +7845,7 @@
     </row>
     <row r="245" spans="1:26" ht="112.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" s="4" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="L245" t="s">
         <v>22</v>
@@ -7868,7 +7853,7 @@
       <c r="O245" s="4"/>
       <c r="T245" s="1"/>
       <c r="U245" s="5" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="V245" s="4" t="s">
         <v>276</v>
@@ -7883,7 +7868,7 @@
     </row>
     <row r="246" spans="1:26" ht="112.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A246" s="4" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="L246" t="s">
         <v>22</v>
@@ -7891,7 +7876,7 @@
       <c r="O246" s="4"/>
       <c r="T246" s="1"/>
       <c r="U246" s="5" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="V246" s="4" t="s">
         <v>276</v>
@@ -7906,7 +7891,7 @@
     </row>
     <row r="247" spans="1:26" ht="112.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A247" s="4" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="L247" t="s">
         <v>22</v>
@@ -7914,7 +7899,7 @@
       <c r="O247" s="4"/>
       <c r="T247" s="1"/>
       <c r="U247" s="5" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="V247" s="4" t="s">
         <v>276</v>
@@ -7929,7 +7914,7 @@
     </row>
     <row r="248" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A248" s="4" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="F248" s="4" t="s">
         <v>22</v>
@@ -7953,7 +7938,7 @@
     </row>
     <row r="249" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A249" s="4" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="F249" s="4" t="s">
         <v>22</v>
@@ -7977,7 +7962,7 @@
     </row>
     <row r="250" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A250" s="4" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="F250" s="4" t="s">
         <v>22</v>
@@ -8001,7 +7986,7 @@
     </row>
     <row r="251" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A251" s="4" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="F251" s="4" t="s">
         <v>22</v>
@@ -8025,7 +8010,7 @@
     </row>
     <row r="252" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A252" s="4" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="E252" s="4" t="s">
         <v>22</v>
@@ -8049,7 +8034,7 @@
     </row>
     <row r="253" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A253" s="4" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="E253" s="4" t="s">
         <v>22</v>
@@ -8073,7 +8058,7 @@
     </row>
     <row r="254" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A254" s="4" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="E254" s="4" t="s">
         <v>22</v>
@@ -8097,7 +8082,7 @@
     </row>
     <row r="255" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A255" s="4" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="E255" s="4" t="s">
         <v>22</v>
@@ -8121,7 +8106,7 @@
     </row>
     <row r="256" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A256" s="4" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="E256" s="4" t="s">
         <v>22</v>
@@ -8148,7 +8133,7 @@
     </row>
     <row r="257" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A257" s="4" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="E257" s="4" t="s">
         <v>22</v>
@@ -8175,7 +8160,7 @@
     </row>
     <row r="258" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A258" s="4" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="E258" s="4" t="s">
         <v>22</v>
@@ -8202,7 +8187,7 @@
     </row>
     <row r="259" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A259" s="4" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="E259" s="4" t="s">
         <v>22</v>
@@ -8237,7 +8222,7 @@
     </row>
     <row r="261" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A261" s="4" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="I261" t="s">
         <v>22</v>
@@ -8260,7 +8245,7 @@
     </row>
     <row r="262" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A262" s="4" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="I262" t="s">
         <v>22</v>
@@ -8283,7 +8268,7 @@
     </row>
     <row r="263" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A263" s="4" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="I263" t="s">
         <v>22</v>
@@ -8306,7 +8291,7 @@
     </row>
     <row r="264" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A264" s="4" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="I264" t="s">
         <v>22</v>
@@ -8337,7 +8322,7 @@
     </row>
     <row r="266" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A266" s="4" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="I266" t="s">
         <v>22</v>
@@ -8360,7 +8345,7 @@
     </row>
     <row r="267" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A267" s="4" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="I267" t="s">
         <v>22</v>
@@ -8383,7 +8368,7 @@
     </row>
     <row r="268" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A268" s="4" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="I268" t="s">
         <v>22</v>
@@ -8406,7 +8391,7 @@
     </row>
     <row r="269" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A269" s="4" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="I269" t="s">
         <v>22</v>
@@ -8437,7 +8422,7 @@
     </row>
     <row r="271" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A271" s="4" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="M271" t="s">
         <v>22</v>
@@ -8458,7 +8443,7 @@
     </row>
     <row r="272" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A272" s="4" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="M272" t="s">
         <v>22</v>
@@ -8479,7 +8464,7 @@
     </row>
     <row r="273" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A273" s="4" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="M273" t="s">
         <v>22</v>
@@ -8500,7 +8485,7 @@
     </row>
     <row r="274" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A274" s="4" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="M274" t="s">
         <v>22</v>
@@ -8563,7 +8548,7 @@
     </row>
     <row r="278" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A278" s="4" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="I278" t="s">
         <v>22</v>
@@ -8597,7 +8582,7 @@
     </row>
     <row r="279" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A279" s="4" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="I279" t="s">
         <v>22</v>
@@ -8631,7 +8616,7 @@
     </row>
     <row r="280" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A280" s="4" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="I280" t="s">
         <v>22</v>
@@ -8665,7 +8650,7 @@
     </row>
     <row r="281" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A281" s="4" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="I281" t="s">
         <v>22</v>
@@ -8707,7 +8692,7 @@
     </row>
     <row r="283" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A283" s="4" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="B283" s="4" t="s">
         <v>22</v>
@@ -8736,7 +8721,7 @@
     </row>
     <row r="284" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A284" s="4" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="B284" s="4" t="s">
         <v>22</v>
@@ -8765,7 +8750,7 @@
     </row>
     <row r="285" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A285" s="4" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="B285" s="4" t="s">
         <v>22</v>
@@ -8794,7 +8779,7 @@
     </row>
     <row r="286" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A286" s="4" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="B286" s="4" t="s">
         <v>22</v>
@@ -8831,7 +8816,7 @@
     </row>
     <row r="288" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A288" s="4" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="M288" t="s">
         <v>22</v>
@@ -8851,7 +8836,7 @@
     </row>
     <row r="289" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A289" s="4" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="M289" t="s">
         <v>22</v>
@@ -8871,7 +8856,7 @@
     </row>
     <row r="290" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A290" s="4" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="M290" t="s">
         <v>22</v>
@@ -8891,7 +8876,7 @@
     </row>
     <row r="291" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A291" s="4" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="M291" t="s">
         <v>22</v>
@@ -8911,7 +8896,7 @@
     </row>
     <row r="292" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A292" s="4" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="B292" s="4" t="s">
         <v>22</v>
@@ -8940,7 +8925,7 @@
     </row>
     <row r="293" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A293" s="4" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="B293" s="4" t="s">
         <v>22</v>
@@ -8969,7 +8954,7 @@
     </row>
     <row r="294" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A294" s="4" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="B294" s="4" t="s">
         <v>22</v>
@@ -8998,7 +8983,7 @@
     </row>
     <row r="295" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A295" s="4" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="B295" s="4" t="s">
         <v>22</v>
@@ -9498,19 +9483,19 @@
         <v>25</v>
       </c>
       <c r="O1" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="P1" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="Q1" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="R1" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="S1" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="T1" t="s">
         <v>13</v>
@@ -10125,225 +10110,172 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C6A530-5E3B-DF44-97F6-49A96DE68D54}">
   <sheetPr codeName="Blad5"/>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" s="1">
+        <v>100</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>330</v>
+      </c>
+      <c r="B3" s="1">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>331</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>332</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>333</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C6" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>334</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>335</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>336</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>331</v>
-      </c>
-      <c r="B5" s="1">
-        <v>100</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>332</v>
-      </c>
-      <c r="B6" s="1">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>333</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="D7" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>334</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="D8" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>335</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>351</v>
-      </c>
       <c r="C9" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="D9" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="D10" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="D11" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="D12" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="D13" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="D14" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>341</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="D15" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>342</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="D16" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>343</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="D17" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
-        <v>345</v>
-      </c>
+        <v>346</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="B7:C17" numberStoredAsText="1"/>
+    <ignoredError sqref="B4:C14" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
poging tot over de dag plannen, mislukt
</commit_message>
<xml_diff>
--- a/MODPRdataset.xlsx
+++ b/MODPRdataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robbert\Github\Modelleren\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC5A51F7-83E0-43AE-BCBE-77E4BE29BE7F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F46F31E-6DFD-46E0-A799-04E7384977E8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{24CE0B4A-80F4-8A44-8D6D-9FAD261C3CF8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{24CE0B4A-80F4-8A44-8D6D-9FAD261C3CF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Project tasks" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1495" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1552" uniqueCount="377">
   <si>
     <t>Task</t>
   </si>
@@ -1178,6 +1178,15 @@
   </si>
   <si>
     <t>troubleshooting</t>
+  </si>
+  <si>
+    <t>Extra 1</t>
+  </si>
+  <si>
+    <t>Extra 2</t>
+  </si>
+  <si>
+    <t>Extra 3</t>
   </si>
 </sst>
 </file>
@@ -3391,7 +3400,7 @@
   <sheetPr codeName="Blad2"/>
   <dimension ref="A1:AG284"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="S228" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -13361,9 +13370,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08EA75A-4C53-5041-B680-B852EC61F73B}">
   <sheetPr codeName="Blad3"/>
-  <dimension ref="A1:T14"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -13900,6 +13911,183 @@
         <v>18</v>
       </c>
       <c r="S14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>374</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" t="s">
+        <v>18</v>
+      </c>
+      <c r="K15" t="s">
+        <v>18</v>
+      </c>
+      <c r="L15" t="s">
+        <v>18</v>
+      </c>
+      <c r="M15" t="s">
+        <v>18</v>
+      </c>
+      <c r="N15" t="s">
+        <v>18</v>
+      </c>
+      <c r="O15" t="s">
+        <v>18</v>
+      </c>
+      <c r="P15" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>18</v>
+      </c>
+      <c r="R15" t="s">
+        <v>18</v>
+      </c>
+      <c r="S15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>375</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" t="s">
+        <v>18</v>
+      </c>
+      <c r="K16" t="s">
+        <v>18</v>
+      </c>
+      <c r="L16" t="s">
+        <v>18</v>
+      </c>
+      <c r="M16" t="s">
+        <v>18</v>
+      </c>
+      <c r="N16" t="s">
+        <v>18</v>
+      </c>
+      <c r="O16" t="s">
+        <v>18</v>
+      </c>
+      <c r="P16" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>18</v>
+      </c>
+      <c r="R16" t="s">
+        <v>18</v>
+      </c>
+      <c r="S16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>376</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" t="s">
+        <v>18</v>
+      </c>
+      <c r="K17" t="s">
+        <v>18</v>
+      </c>
+      <c r="L17" t="s">
+        <v>18</v>
+      </c>
+      <c r="M17" t="s">
+        <v>18</v>
+      </c>
+      <c r="N17" t="s">
+        <v>18</v>
+      </c>
+      <c r="O17" t="s">
+        <v>18</v>
+      </c>
+      <c r="P17" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>18</v>
+      </c>
+      <c r="R17" t="s">
+        <v>18</v>
+      </c>
+      <c r="S17" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
nog een ding en dan moet het klaar zijn...haha
</commit_message>
<xml_diff>
--- a/MODPRdataset.xlsx
+++ b/MODPRdataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robbert\Github\Modelleren\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE732BD-57C3-4A8A-A5F3-C99A9A305EDA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20ACF7A3-0E36-4E05-97CD-7ED530B8F108}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{24CE0B4A-80F4-8A44-8D6D-9FAD261C3CF8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{24CE0B4A-80F4-8A44-8D6D-9FAD261C3CF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Project tasks" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1552" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1530" uniqueCount="361">
   <si>
     <t>Task</t>
   </si>
@@ -1048,42 +1048,6 @@
 can only be done whenever prep check-up during sprint is completed</t>
   </si>
   <si>
-    <t>special troubleshooting 1.1</t>
-  </si>
-  <si>
-    <t>special troubleshooting 2.1</t>
-  </si>
-  <si>
-    <t>special troubleshooting 3.1</t>
-  </si>
-  <si>
-    <t>special troubleshooting 4.1</t>
-  </si>
-  <si>
-    <t>special troubleshooting 1.2</t>
-  </si>
-  <si>
-    <t>special troubleshooting 2.2</t>
-  </si>
-  <si>
-    <t>special troubleshooting 3.2</t>
-  </si>
-  <si>
-    <t>special troubleshooting 4.2</t>
-  </si>
-  <si>
-    <t>special troubleshooting 1.3</t>
-  </si>
-  <si>
-    <t>special troubleshooting 2.3</t>
-  </si>
-  <si>
-    <t>special troubleshooting 3.3</t>
-  </si>
-  <si>
-    <t>special troubleshooting 4.3</t>
-  </si>
-  <si>
     <t>DurationExp.1</t>
   </si>
   <si>
@@ -1166,6 +1130,15 @@
   </si>
   <si>
     <t>check-up 2</t>
+  </si>
+  <si>
+    <t>special troubleshooting 1</t>
+  </si>
+  <si>
+    <t>special troubleshooting 2</t>
+  </si>
+  <si>
+    <t>special troubleshooting 3</t>
   </si>
 </sst>
 </file>
@@ -3379,11 +3352,11 @@
   <sheetPr codeName="Blad2"/>
   <dimension ref="A1:AG280"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B195" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B214" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A201" sqref="A201"/>
+      <selection pane="bottomRight" activeCell="A214" sqref="A214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3467,31 +3440,31 @@
         <v>233</v>
       </c>
       <c r="V1" s="7" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="W1" s="7" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="X1" s="7" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="Y1" s="7" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
       <c r="Z1" s="7" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="AA1" s="7" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="AB1" s="7" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="AC1" s="7" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
       <c r="AD1" s="7" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
       <c r="AE1" s="7" t="s">
         <v>3</v>
@@ -3612,7 +3585,7 @@
         <v>18</v>
       </c>
       <c r="U5" s="4" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="V5" s="7">
         <v>3</v>
@@ -6307,7 +6280,7 @@
         <v>18</v>
       </c>
       <c r="U86" s="4" t="s">
-        <v>352</v>
+        <v>340</v>
       </c>
       <c r="V86" s="7">
         <v>6</v>
@@ -8631,7 +8604,7 @@
         <v>18</v>
       </c>
       <c r="U159" s="4" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="V159" s="7">
         <v>4</v>
@@ -9041,7 +9014,7 @@
         <v>18</v>
       </c>
       <c r="U171" s="4" t="s">
-        <v>354</v>
+        <v>342</v>
       </c>
       <c r="V171" s="7">
         <v>4</v>
@@ -9357,7 +9330,7 @@
         <v>18</v>
       </c>
       <c r="U181" s="4" t="s">
-        <v>355</v>
+        <v>343</v>
       </c>
       <c r="V181" s="7">
         <v>2</v>
@@ -9659,7 +9632,7 @@
     </row>
     <row r="191" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A191" s="4" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
       <c r="K191" t="s">
         <v>18</v>
@@ -9708,7 +9681,7 @@
     </row>
     <row r="192" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A192" s="4" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
       <c r="K192" t="s">
         <v>18</v>
@@ -9757,7 +9730,7 @@
     </row>
     <row r="193" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A193" s="4" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
       <c r="K193" t="s">
         <v>18</v>
@@ -9806,7 +9779,7 @@
     </row>
     <row r="194" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A194" s="4" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
       <c r="K194" t="s">
         <v>18</v>
@@ -9855,7 +9828,7 @@
     </row>
     <row r="195" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A195" s="4" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="K195" t="s">
         <v>18</v>
@@ -9893,7 +9866,7 @@
     </row>
     <row r="196" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A196" s="4" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="K196" t="s">
         <v>18</v>
@@ -9931,7 +9904,7 @@
     </row>
     <row r="197" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A197" s="4" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="K197" t="s">
         <v>18</v>
@@ -9969,7 +9942,7 @@
     </row>
     <row r="198" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A198" s="4" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="K198" t="s">
         <v>18</v>
@@ -10007,7 +9980,7 @@
     </row>
     <row r="199" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A199" s="4" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
       <c r="K199" t="s">
         <v>18</v>
@@ -10048,7 +10021,7 @@
     </row>
     <row r="200" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A200" s="4" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
       <c r="K200" t="s">
         <v>18</v>
@@ -10089,7 +10062,7 @@
     </row>
     <row r="201" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A201" s="4" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
       <c r="K201" t="s">
         <v>18</v>
@@ -10130,7 +10103,7 @@
     </row>
     <row r="202" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A202" s="4" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
       <c r="K202" t="s">
         <v>18</v>
@@ -10184,7 +10157,7 @@
     </row>
     <row r="204" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A204" s="4" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="K204" t="s">
         <v>18</v>
@@ -10229,7 +10202,7 @@
     </row>
     <row r="205" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A205" s="4" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="K205" t="s">
         <v>18</v>
@@ -10274,7 +10247,7 @@
     </row>
     <row r="206" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A206" s="4" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="K206" t="s">
         <v>18</v>
@@ -10319,7 +10292,7 @@
     </row>
     <row r="207" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A207" s="4" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="K207" t="s">
         <v>18</v>
@@ -10364,7 +10337,7 @@
     </row>
     <row r="208" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A208" s="4" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="K208" t="s">
         <v>18</v>
@@ -10411,7 +10384,7 @@
     </row>
     <row r="209" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A209" s="4" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="K209" t="s">
         <v>18</v>
@@ -10458,7 +10431,7 @@
     </row>
     <row r="210" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A210" s="4" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="K210" t="s">
         <v>18</v>
@@ -10505,7 +10478,7 @@
     </row>
     <row r="211" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A211" s="4" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="K211" t="s">
         <v>18</v>
@@ -10552,7 +10525,7 @@
     </row>
     <row r="212" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A212" s="4" t="s">
-        <v>330</v>
+        <v>358</v>
       </c>
       <c r="F212" s="4" t="s">
         <v>18</v>
@@ -10593,7 +10566,7 @@
     </row>
     <row r="213" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A213" s="4" t="s">
-        <v>331</v>
+        <v>358</v>
       </c>
       <c r="F213" s="4" t="s">
         <v>18</v>
@@ -10634,7 +10607,7 @@
     </row>
     <row r="214" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A214" s="4" t="s">
-        <v>332</v>
+        <v>358</v>
       </c>
       <c r="F214" s="4" t="s">
         <v>18</v>
@@ -10675,7 +10648,7 @@
     </row>
     <row r="215" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A215" s="4" t="s">
-        <v>333</v>
+        <v>358</v>
       </c>
       <c r="F215" s="4" t="s">
         <v>18</v>
@@ -10716,7 +10689,7 @@
     </row>
     <row r="216" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A216" s="4" t="s">
-        <v>334</v>
+        <v>359</v>
       </c>
       <c r="E216" s="4" t="s">
         <v>18</v>
@@ -10757,7 +10730,7 @@
     </row>
     <row r="217" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A217" s="4" t="s">
-        <v>335</v>
+        <v>359</v>
       </c>
       <c r="E217" s="4" t="s">
         <v>18</v>
@@ -10798,7 +10771,7 @@
     </row>
     <row r="218" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A218" s="4" t="s">
-        <v>336</v>
+        <v>359</v>
       </c>
       <c r="E218" s="4" t="s">
         <v>18</v>
@@ -10839,7 +10812,7 @@
     </row>
     <row r="219" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A219" s="4" t="s">
-        <v>337</v>
+        <v>359</v>
       </c>
       <c r="E219" s="4" t="s">
         <v>18</v>
@@ -10880,7 +10853,7 @@
     </row>
     <row r="220" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A220" s="4" t="s">
-        <v>338</v>
+        <v>360</v>
       </c>
       <c r="E220" s="4" t="s">
         <v>18</v>
@@ -10924,7 +10897,7 @@
     </row>
     <row r="221" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A221" s="4" t="s">
-        <v>339</v>
+        <v>360</v>
       </c>
       <c r="E221" s="4" t="s">
         <v>18</v>
@@ -10968,7 +10941,7 @@
     </row>
     <row r="222" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A222" s="4" t="s">
-        <v>340</v>
+        <v>360</v>
       </c>
       <c r="E222" s="4" t="s">
         <v>18</v>
@@ -11012,7 +10985,7 @@
     </row>
     <row r="223" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A223" s="4" t="s">
-        <v>341</v>
+        <v>360</v>
       </c>
       <c r="E223" s="4" t="s">
         <v>18</v>
@@ -11068,7 +11041,7 @@
     </row>
     <row r="225" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A225" s="4" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="I225" t="s">
         <v>18</v>
@@ -11112,7 +11085,7 @@
     </row>
     <row r="226" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A226" s="4" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="I226" t="s">
         <v>18</v>
@@ -11156,7 +11129,7 @@
     </row>
     <row r="227" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A227" s="4" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="I227" t="s">
         <v>18</v>
@@ -11200,7 +11173,7 @@
     </row>
     <row r="228" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A228" s="4" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="I228" t="s">
         <v>18</v>
@@ -11256,7 +11229,7 @@
     </row>
     <row r="230" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A230" s="4" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="I230" t="s">
         <v>18</v>
@@ -11300,7 +11273,7 @@
     </row>
     <row r="231" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A231" s="4" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="I231" t="s">
         <v>18</v>
@@ -11344,7 +11317,7 @@
     </row>
     <row r="232" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A232" s="4" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="I232" t="s">
         <v>18</v>
@@ -11388,7 +11361,7 @@
     </row>
     <row r="233" spans="1:33" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A233" s="4" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="I233" t="s">
         <v>18</v>
@@ -11444,7 +11417,7 @@
     </row>
     <row r="235" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A235" s="4" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="M235" t="s">
         <v>18</v>
@@ -11486,7 +11459,7 @@
     </row>
     <row r="236" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A236" s="4" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="M236" t="s">
         <v>18</v>
@@ -11528,7 +11501,7 @@
     </row>
     <row r="237" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A237" s="4" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="M237" t="s">
         <v>18</v>
@@ -11570,7 +11543,7 @@
     </row>
     <row r="238" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A238" s="4" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="M238" t="s">
         <v>18</v>
@@ -11680,7 +11653,7 @@
     </row>
     <row r="242" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A242" s="4" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
       <c r="I242" t="s">
         <v>18</v>
@@ -11735,7 +11708,7 @@
     </row>
     <row r="243" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A243" s="4" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
       <c r="I243" t="s">
         <v>18</v>
@@ -11790,7 +11763,7 @@
     </row>
     <row r="244" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A244" s="4" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
       <c r="I244" t="s">
         <v>18</v>
@@ -11845,7 +11818,7 @@
     </row>
     <row r="245" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A245" s="4" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
       <c r="I245" t="s">
         <v>18</v>
@@ -11912,7 +11885,7 @@
     </row>
     <row r="247" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A247" s="4" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="B247" s="4" t="s">
         <v>18</v>
@@ -11962,7 +11935,7 @@
     </row>
     <row r="248" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A248" s="4" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="B248" s="4" t="s">
         <v>18</v>
@@ -12012,7 +11985,7 @@
     </row>
     <row r="249" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A249" s="4" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="B249" s="4" t="s">
         <v>18</v>
@@ -12062,7 +12035,7 @@
     </row>
     <row r="250" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A250" s="4" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="B250" s="4" t="s">
         <v>18</v>
@@ -12124,7 +12097,7 @@
     </row>
     <row r="252" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A252" s="4" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
       <c r="B252" s="4" t="s">
         <v>18</v>
@@ -12177,7 +12150,7 @@
     </row>
     <row r="253" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A253" s="4" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
       <c r="B253" s="4" t="s">
         <v>18</v>
@@ -12230,7 +12203,7 @@
     </row>
     <row r="254" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A254" s="4" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
       <c r="B254" s="4" t="s">
         <v>18</v>
@@ -12283,7 +12256,7 @@
     </row>
     <row r="255" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A255" s="4" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
       <c r="B255" s="4" t="s">
         <v>18</v>
@@ -13199,7 +13172,9 @@
   <sheetPr codeName="Blad3"/>
   <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17:N17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -13741,7 +13716,7 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
@@ -13759,27 +13734,6 @@
         <v>18</v>
       </c>
       <c r="G15" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" t="s">
-        <v>18</v>
-      </c>
-      <c r="I15" t="s">
-        <v>18</v>
-      </c>
-      <c r="J15" t="s">
-        <v>18</v>
-      </c>
-      <c r="K15" t="s">
-        <v>18</v>
-      </c>
-      <c r="L15" t="s">
-        <v>18</v>
-      </c>
-      <c r="M15" t="s">
-        <v>18</v>
-      </c>
-      <c r="N15" t="s">
         <v>18</v>
       </c>
       <c r="O15" t="s">
@@ -13800,25 +13754,7 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>366</v>
-      </c>
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" t="s">
-        <v>18</v>
+        <v>354</v>
       </c>
       <c r="H16" t="s">
         <v>18</v>
@@ -13859,17 +13795,11 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>367</v>
-      </c>
-      <c r="B17" t="s">
-        <v>18</v>
+        <v>355</v>
       </c>
       <c r="C17" t="s">
         <v>18</v>
       </c>
-      <c r="D17" t="s">
-        <v>18</v>
-      </c>
       <c r="E17" t="s">
         <v>18</v>
       </c>
@@ -13877,27 +13807,6 @@
         <v>18</v>
       </c>
       <c r="G17" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" t="s">
-        <v>18</v>
-      </c>
-      <c r="I17" t="s">
-        <v>18</v>
-      </c>
-      <c r="J17" t="s">
-        <v>18</v>
-      </c>
-      <c r="K17" t="s">
-        <v>18</v>
-      </c>
-      <c r="L17" t="s">
-        <v>18</v>
-      </c>
-      <c r="M17" t="s">
-        <v>18</v>
-      </c>
-      <c r="N17" t="s">
         <v>18</v>
       </c>
       <c r="O17" t="s">

</xml_diff>